<commit_message>
revisi input data pengguna alumni
</commit_message>
<xml_diff>
--- a/rekap hasil kuesioner alumni.xlsx
+++ b/rekap hasil kuesioner alumni.xlsx
@@ -5,19 +5,20 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kuliah\SM 8\SPS\Tracer Study\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\siluni-ts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCB6BB80-FA9C-47A2-A0C1-3ADDD54A4A2C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E934FFBE-3C7F-42EA-8DAB-9247E63C7DAC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8934060E-9541-45B4-8186-CE18E30F50FB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{8934060E-9541-45B4-8186-CE18E30F50FB}"/>
   </bookViews>
   <sheets>
     <sheet name="eqi" sheetId="1" r:id="rId1"/>
-    <sheet name="kak acil" sheetId="2" r:id="rId2"/>
-    <sheet name="kak ferdi" sheetId="3" r:id="rId3"/>
-    <sheet name="kak tiara" sheetId="5" r:id="rId4"/>
-    <sheet name="kak anita" sheetId="4" r:id="rId5"/>
+    <sheet name="Kak rahmi" sheetId="6" r:id="rId2"/>
+    <sheet name="kak acil" sheetId="2" r:id="rId3"/>
+    <sheet name="kak ferdi" sheetId="3" r:id="rId4"/>
+    <sheet name="kak tiara" sheetId="5" r:id="rId5"/>
+    <sheet name="kak anita" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="144">
   <si>
     <t>M Nurilman Baehaqi</t>
   </si>
@@ -446,6 +447,30 @@
   </si>
   <si>
     <t>Terus belajar!</t>
+  </si>
+  <si>
+    <t>Rahmi Putri</t>
+  </si>
+  <si>
+    <t>5 bulan</t>
+  </si>
+  <si>
+    <t>50-100</t>
+  </si>
+  <si>
+    <t>9 Semester</t>
+  </si>
+  <si>
+    <t>abstrak dipukblikasikan pada jkoma (jurnal ilmu komputer dan aplikasi) http://journal.unj.ac.id/unj/index.php/jkoma/article/view/6496</t>
+  </si>
+  <si>
+    <t>web development</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>saran saya, mahasiswa diikutsertakan dalam project untuk mengetahui gambaran kerja serta juga dapat meningkatkan skill problem solving.</t>
   </si>
 </sst>
 </file>
@@ -641,7 +666,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -691,6 +716,40 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -700,28 +759,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -730,32 +777,22 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -764,16 +801,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1372,7 +1403,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CAE5304-FEA1-4381-AF1C-BCABE511D221}">
   <dimension ref="A1:J90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+    <sheetView topLeftCell="A67" workbookViewId="0">
       <selection activeCell="B94" sqref="B94"/>
     </sheetView>
   </sheetViews>
@@ -1393,140 +1424,140 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="18"/>
+      <c r="C2" s="30"/>
     </row>
     <row r="3" spans="1:3" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
     </row>
     <row r="4" spans="1:3" ht="26.25" thickBot="1">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="17"/>
+      <c r="C4" s="29"/>
     </row>
     <row r="5" spans="1:3" ht="26.25" thickBot="1">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="17"/>
+      <c r="C5" s="29"/>
     </row>
     <row r="6" spans="1:3" ht="15.75" thickBot="1">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="17"/>
+      <c r="C6" s="29"/>
     </row>
     <row r="7" spans="1:3" ht="26.25" thickBot="1">
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="17"/>
+      <c r="C7" s="29"/>
     </row>
     <row r="8" spans="1:3" ht="26.25" thickBot="1">
       <c r="A8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="17">
+      <c r="B8" s="29">
         <v>5</v>
       </c>
-      <c r="C8" s="17"/>
+      <c r="C8" s="29"/>
     </row>
     <row r="9" spans="1:3" ht="26.25" thickBot="1">
       <c r="A9" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="17">
+      <c r="B9" s="29">
         <v>3</v>
       </c>
-      <c r="C9" s="17"/>
+      <c r="C9" s="29"/>
     </row>
     <row r="10" spans="1:3" ht="26.25" thickBot="1">
       <c r="A10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="17"/>
+      <c r="C10" s="29"/>
     </row>
     <row r="11" spans="1:3" ht="137.25" customHeight="1">
-      <c r="A11" s="20" t="s">
+      <c r="A11" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="20"/>
+      <c r="C11" s="25"/>
     </row>
     <row r="12" spans="1:3" ht="51" customHeight="1" thickBot="1">
-      <c r="A12" s="21"/>
-      <c r="B12" s="21" t="s">
+      <c r="A12" s="27"/>
+      <c r="B12" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="21"/>
+      <c r="C12" s="27"/>
     </row>
     <row r="13" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A13" s="22" t="s">
+      <c r="A13" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="22"/>
-      <c r="C13" s="22"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="28"/>
     </row>
     <row r="14" spans="1:3" ht="15.75" thickBot="1">
       <c r="A14" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="17"/>
+      <c r="C14" s="29"/>
     </row>
     <row r="15" spans="1:3" ht="15.75" thickBot="1">
       <c r="A15" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="17"/>
+      <c r="C15" s="29"/>
     </row>
     <row r="16" spans="1:3" ht="60.75" customHeight="1">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="20"/>
+      <c r="C16" s="25"/>
     </row>
     <row r="17" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A17" s="21"/>
-      <c r="B17" s="21" t="s">
+      <c r="A17" s="27"/>
+      <c r="B17" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="21"/>
+      <c r="C17" s="27"/>
     </row>
     <row r="18" spans="1:3" ht="29.25" customHeight="1" thickBot="1">
-      <c r="A18" s="20" t="s">
+      <c r="A18" s="25" t="s">
         <v>26</v>
       </c>
       <c r="B18" s="4" t="s">
@@ -1537,7 +1568,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A19" s="23"/>
+      <c r="A19" s="26"/>
       <c r="B19" s="4" t="s">
         <v>29</v>
       </c>
@@ -1546,7 +1577,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A20" s="23"/>
+      <c r="A20" s="26"/>
       <c r="B20" s="4" t="s">
         <v>31</v>
       </c>
@@ -1555,7 +1586,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A21" s="23"/>
+      <c r="A21" s="26"/>
       <c r="B21" s="4" t="s">
         <v>33</v>
       </c>
@@ -1564,7 +1595,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A22" s="23"/>
+      <c r="A22" s="26"/>
       <c r="B22" s="4" t="s">
         <v>34</v>
       </c>
@@ -1573,7 +1604,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A23" s="23"/>
+      <c r="A23" s="26"/>
       <c r="B23" s="4" t="s">
         <v>35</v>
       </c>
@@ -1582,7 +1613,7 @@
       </c>
     </row>
     <row r="24" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A24" s="21"/>
+      <c r="A24" s="27"/>
       <c r="B24" s="4" t="s">
         <v>36</v>
       </c>
@@ -1594,73 +1625,73 @@
       <c r="A25" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B25" s="17" t="s">
+      <c r="B25" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="C25" s="17"/>
+      <c r="C25" s="29"/>
     </row>
     <row r="26" spans="1:3" ht="15.75" thickBot="1">
       <c r="A26" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B26" s="17"/>
-      <c r="C26" s="17"/>
+      <c r="B26" s="29"/>
+      <c r="C26" s="29"/>
     </row>
     <row r="27" spans="1:3" ht="15.75" thickBot="1">
       <c r="A27" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B27" s="17"/>
-      <c r="C27" s="17"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="29"/>
     </row>
     <row r="28" spans="1:3" ht="124.5" customHeight="1">
-      <c r="A28" s="20" t="s">
+      <c r="A28" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="B28" s="20" t="s">
+      <c r="B28" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="C28" s="20"/>
+      <c r="C28" s="25"/>
     </row>
     <row r="29" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A29" s="21"/>
-      <c r="B29" s="21" t="s">
+      <c r="A29" s="27"/>
+      <c r="B29" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="C29" s="21"/>
+      <c r="C29" s="27"/>
     </row>
     <row r="30" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A30" s="22" t="s">
+      <c r="A30" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="B30" s="22"/>
-      <c r="C30" s="22"/>
+      <c r="B30" s="28"/>
+      <c r="C30" s="28"/>
     </row>
     <row r="31" spans="1:3" ht="26.25" thickBot="1">
       <c r="A31" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B31" s="17" t="s">
+      <c r="B31" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="C31" s="17"/>
+      <c r="C31" s="29"/>
     </row>
     <row r="32" spans="1:3" ht="26.25" thickBot="1">
       <c r="A32" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B32" s="17"/>
-      <c r="C32" s="17"/>
+      <c r="B32" s="29"/>
+      <c r="C32" s="29"/>
     </row>
     <row r="33" spans="1:3" ht="15.75" thickBot="1">
       <c r="A33" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B33" s="17"/>
-      <c r="C33" s="17"/>
+      <c r="B33" s="29"/>
+      <c r="C33" s="29"/>
     </row>
     <row r="34" spans="1:3" ht="26.25" thickBot="1">
-      <c r="A34" s="20" t="s">
+      <c r="A34" s="25" t="s">
         <v>49</v>
       </c>
       <c r="B34" s="4" t="s">
@@ -1669,258 +1700,258 @@
       <c r="C34" s="5"/>
     </row>
     <row r="35" spans="1:3" ht="26.25" thickBot="1">
-      <c r="A35" s="23"/>
+      <c r="A35" s="26"/>
       <c r="B35" s="4" t="s">
         <v>51</v>
       </c>
       <c r="C35" s="5"/>
     </row>
     <row r="36" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A36" s="23"/>
+      <c r="A36" s="26"/>
       <c r="B36" s="4" t="s">
         <v>52</v>
       </c>
       <c r="C36" s="5"/>
     </row>
     <row r="37" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A37" s="23"/>
+      <c r="A37" s="26"/>
       <c r="B37" s="4" t="s">
         <v>53</v>
       </c>
       <c r="C37" s="5"/>
     </row>
     <row r="38" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A38" s="23"/>
+      <c r="A38" s="26"/>
       <c r="B38" s="4" t="s">
         <v>54</v>
       </c>
       <c r="C38" s="5"/>
     </row>
     <row r="39" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A39" s="23"/>
+      <c r="A39" s="26"/>
       <c r="B39" s="4" t="s">
         <v>55</v>
       </c>
       <c r="C39" s="5"/>
     </row>
     <row r="40" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A40" s="23"/>
+      <c r="A40" s="26"/>
       <c r="B40" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C40" s="5"/>
     </row>
     <row r="41" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A41" s="23"/>
+      <c r="A41" s="26"/>
       <c r="B41" s="4" t="s">
         <v>57</v>
       </c>
       <c r="C41" s="5"/>
     </row>
     <row r="42" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A42" s="23"/>
+      <c r="A42" s="26"/>
       <c r="B42" s="4" t="s">
         <v>58</v>
       </c>
       <c r="C42" s="5"/>
     </row>
     <row r="43" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A43" s="23"/>
+      <c r="A43" s="26"/>
       <c r="B43" s="4" t="s">
         <v>59</v>
       </c>
       <c r="C43" s="5"/>
     </row>
     <row r="44" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A44" s="23"/>
+      <c r="A44" s="26"/>
       <c r="B44" s="4" t="s">
         <v>60</v>
       </c>
       <c r="C44" s="5"/>
     </row>
     <row r="45" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A45" s="23"/>
+      <c r="A45" s="26"/>
       <c r="B45" s="4" t="s">
         <v>61</v>
       </c>
       <c r="C45" s="5"/>
     </row>
     <row r="46" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A46" s="23"/>
+      <c r="A46" s="26"/>
       <c r="B46" s="4" t="s">
         <v>62</v>
       </c>
       <c r="C46" s="5"/>
     </row>
     <row r="47" spans="1:3" ht="26.25" thickBot="1">
-      <c r="A47" s="23"/>
+      <c r="A47" s="26"/>
       <c r="B47" s="4" t="s">
         <v>63</v>
       </c>
       <c r="C47" s="5"/>
     </row>
     <row r="48" spans="1:3" ht="26.25" thickBot="1">
-      <c r="A48" s="23"/>
+      <c r="A48" s="26"/>
       <c r="B48" s="4" t="s">
         <v>64</v>
       </c>
       <c r="C48" s="5"/>
     </row>
     <row r="49" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A49" s="23"/>
+      <c r="A49" s="26"/>
       <c r="B49" s="4" t="s">
         <v>65</v>
       </c>
       <c r="C49" s="5"/>
     </row>
     <row r="50" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A50" s="23"/>
+      <c r="A50" s="26"/>
       <c r="B50" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C50" s="5"/>
     </row>
     <row r="51" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A51" s="23"/>
+      <c r="A51" s="26"/>
       <c r="B51" s="4" t="s">
         <v>67</v>
       </c>
       <c r="C51" s="5"/>
     </row>
     <row r="52" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A52" s="23"/>
+      <c r="A52" s="26"/>
       <c r="B52" s="4" t="s">
         <v>68</v>
       </c>
       <c r="C52" s="5"/>
     </row>
     <row r="53" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A53" s="23"/>
+      <c r="A53" s="26"/>
       <c r="B53" s="4" t="s">
         <v>69</v>
       </c>
       <c r="C53" s="5"/>
     </row>
     <row r="54" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A54" s="23"/>
+      <c r="A54" s="26"/>
       <c r="B54" s="4" t="s">
         <v>70</v>
       </c>
       <c r="C54" s="5"/>
     </row>
     <row r="55" spans="1:3" ht="26.25" thickBot="1">
-      <c r="A55" s="23"/>
+      <c r="A55" s="26"/>
       <c r="B55" s="4" t="s">
         <v>71</v>
       </c>
       <c r="C55" s="5"/>
     </row>
     <row r="56" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A56" s="23"/>
+      <c r="A56" s="26"/>
       <c r="B56" s="4" t="s">
         <v>72</v>
       </c>
       <c r="C56" s="5"/>
     </row>
     <row r="57" spans="1:3" ht="26.25" thickBot="1">
-      <c r="A57" s="23"/>
+      <c r="A57" s="26"/>
       <c r="B57" s="4" t="s">
         <v>73</v>
       </c>
       <c r="C57" s="5"/>
     </row>
     <row r="58" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A58" s="23"/>
+      <c r="A58" s="26"/>
       <c r="B58" s="4" t="s">
         <v>74</v>
       </c>
       <c r="C58" s="5"/>
     </row>
     <row r="59" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A59" s="23"/>
+      <c r="A59" s="26"/>
       <c r="B59" s="4" t="s">
         <v>75</v>
       </c>
       <c r="C59" s="5"/>
     </row>
     <row r="60" spans="1:3" ht="26.25" thickBot="1">
-      <c r="A60" s="23"/>
+      <c r="A60" s="26"/>
       <c r="B60" s="4" t="s">
         <v>76</v>
       </c>
       <c r="C60" s="5"/>
     </row>
     <row r="61" spans="1:3" ht="26.25" thickBot="1">
-      <c r="A61" s="23"/>
+      <c r="A61" s="26"/>
       <c r="B61" s="4" t="s">
         <v>77</v>
       </c>
       <c r="C61" s="5"/>
     </row>
     <row r="62" spans="1:3" ht="26.25" thickBot="1">
-      <c r="A62" s="21"/>
+      <c r="A62" s="27"/>
       <c r="B62" s="4" t="s">
         <v>78</v>
       </c>
       <c r="C62" s="5"/>
     </row>
     <row r="63" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A63" s="22" t="s">
+      <c r="A63" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="B63" s="22"/>
-      <c r="C63" s="22"/>
+      <c r="B63" s="28"/>
+      <c r="C63" s="28"/>
     </row>
     <row r="64" spans="1:3" ht="15.75" thickBot="1">
       <c r="A64" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B64" s="17"/>
-      <c r="C64" s="17"/>
+      <c r="B64" s="29"/>
+      <c r="C64" s="29"/>
     </row>
     <row r="65" spans="1:10" ht="15.75" thickBot="1">
       <c r="A65" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B65" s="17"/>
-      <c r="C65" s="17"/>
+      <c r="B65" s="29"/>
+      <c r="C65" s="29"/>
     </row>
     <row r="66" spans="1:10" ht="15.75" thickBot="1">
       <c r="A66" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B66" s="17"/>
-      <c r="C66" s="17"/>
+      <c r="B66" s="29"/>
+      <c r="C66" s="29"/>
     </row>
     <row r="67" spans="1:10" ht="15.75" thickBot="1">
       <c r="A67" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B67" s="17"/>
-      <c r="C67" s="17"/>
+      <c r="B67" s="29"/>
+      <c r="C67" s="29"/>
     </row>
     <row r="68" spans="1:10" ht="15.75" thickBot="1">
       <c r="A68" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B68" s="17"/>
-      <c r="C68" s="17"/>
+      <c r="B68" s="29"/>
+      <c r="C68" s="29"/>
     </row>
     <row r="69" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A69" s="22" t="s">
+      <c r="A69" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="B69" s="22"/>
-      <c r="C69" s="22"/>
+      <c r="B69" s="28"/>
+      <c r="C69" s="28"/>
     </row>
     <row r="70" spans="1:10" ht="165.75" customHeight="1">
       <c r="A70" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="B70" s="20" t="s">
+      <c r="B70" s="25" t="s">
         <v>87</v>
       </c>
-      <c r="C70" s="20"/>
+      <c r="C70" s="25"/>
     </row>
     <row r="74" spans="1:10" ht="75">
       <c r="A74" s="8" t="s">
@@ -1965,23 +1996,23 @@
       </c>
     </row>
     <row r="80" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A80" s="43" t="s">
+      <c r="A80" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B80" s="44" t="s">
+      <c r="B80" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C80" s="44"/>
+      <c r="C80" s="23"/>
     </row>
     <row r="81" spans="1:3" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A81" s="45" t="s">
+      <c r="A81" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="B81" s="45"/>
-      <c r="C81" s="45"/>
+      <c r="B81" s="24"/>
+      <c r="C81" s="24"/>
     </row>
     <row r="82" spans="1:3" ht="26.25" thickBot="1">
-      <c r="A82" s="20" t="s">
+      <c r="A82" s="25" t="s">
         <v>124</v>
       </c>
       <c r="B82" s="4" t="s">
@@ -1992,7 +2023,7 @@
       </c>
     </row>
     <row r="83" spans="1:3" ht="39" thickBot="1">
-      <c r="A83" s="23"/>
+      <c r="A83" s="26"/>
       <c r="B83" s="4" t="s">
         <v>127</v>
       </c>
@@ -2001,7 +2032,7 @@
       </c>
     </row>
     <row r="84" spans="1:3" ht="26.25" thickBot="1">
-      <c r="A84" s="23"/>
+      <c r="A84" s="26"/>
       <c r="B84" s="4" t="s">
         <v>129</v>
       </c>
@@ -2010,7 +2041,7 @@
       </c>
     </row>
     <row r="85" spans="1:3" ht="26.25" thickBot="1">
-      <c r="A85" s="23"/>
+      <c r="A85" s="26"/>
       <c r="B85" s="4" t="s">
         <v>130</v>
       </c>
@@ -2019,7 +2050,7 @@
       </c>
     </row>
     <row r="86" spans="1:3" ht="26.25" thickBot="1">
-      <c r="A86" s="23"/>
+      <c r="A86" s="26"/>
       <c r="B86" s="4" t="s">
         <v>131</v>
       </c>
@@ -2028,7 +2059,7 @@
       </c>
     </row>
     <row r="87" spans="1:3" ht="26.25" thickBot="1">
-      <c r="A87" s="23"/>
+      <c r="A87" s="26"/>
       <c r="B87" s="4" t="s">
         <v>132</v>
       </c>
@@ -2037,7 +2068,7 @@
       </c>
     </row>
     <row r="88" spans="1:3" ht="26.25" thickBot="1">
-      <c r="A88" s="21"/>
+      <c r="A88" s="27"/>
       <c r="B88" s="4" t="s">
         <v>133</v>
       </c>
@@ -2046,35 +2077,41 @@
       </c>
     </row>
     <row r="89" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A89" s="22" t="s">
+      <c r="A89" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="B89" s="22"/>
-      <c r="C89" s="22"/>
+      <c r="B89" s="28"/>
+      <c r="C89" s="28"/>
     </row>
     <row r="90" spans="1:3">
       <c r="A90" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="B90" s="20" t="s">
+      <c r="B90" s="25" t="s">
         <v>135</v>
       </c>
-      <c r="C90" s="20"/>
+      <c r="C90" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="A81:C81"/>
-    <mergeCell ref="A82:A88"/>
-    <mergeCell ref="A89:C89"/>
-    <mergeCell ref="B90:C90"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="A69:C69"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
     <mergeCell ref="A63:C63"/>
     <mergeCell ref="A18:A24"/>
     <mergeCell ref="B25:C25"/>
@@ -2088,24 +2125,18 @@
     <mergeCell ref="B32:C32"/>
     <mergeCell ref="B33:C33"/>
     <mergeCell ref="A34:A62"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="A69:C69"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="A81:C81"/>
+    <mergeCell ref="A82:A88"/>
+    <mergeCell ref="A89:C89"/>
+    <mergeCell ref="B90:C90"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E74" r:id="rId1" tooltip="ALU3145153280" display="https://srv89.niagahoster.com:2083/cpsess0830536724/3rdparty/phpMyAdmin/sql.php" xr:uid="{AFCF538D-1E1A-4654-8232-D354A2EF5754}"/>
@@ -2116,6 +2147,645 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8664B1C2-5204-4F8F-A97C-3CF19A04A2D8}">
+  <dimension ref="A1:C68"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="34.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="35.25" thickBot="1">
+      <c r="A1" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="27" thickBot="1">
+      <c r="A2" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="30"/>
+    </row>
+    <row r="3" spans="1:3" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A3" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+    </row>
+    <row r="4" spans="1:3" ht="115.5" thickBot="1">
+      <c r="A4" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>137</v>
+      </c>
+      <c r="C4" s="29"/>
+    </row>
+    <row r="5" spans="1:3" ht="166.5" thickBot="1">
+      <c r="A5" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="29"/>
+    </row>
+    <row r="6" spans="1:3" ht="64.5" thickBot="1">
+      <c r="A6" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="29" t="s">
+        <v>96</v>
+      </c>
+      <c r="C6" s="29"/>
+    </row>
+    <row r="7" spans="1:3" ht="230.25" thickBot="1">
+      <c r="A7" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="29" t="s">
+        <v>138</v>
+      </c>
+      <c r="C7" s="29"/>
+    </row>
+    <row r="8" spans="1:3" ht="115.5" thickBot="1">
+      <c r="A8" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="29">
+        <v>5</v>
+      </c>
+      <c r="C8" s="29"/>
+    </row>
+    <row r="9" spans="1:3" ht="141" thickBot="1">
+      <c r="A9" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="29">
+        <v>3</v>
+      </c>
+      <c r="C9" s="29"/>
+    </row>
+    <row r="10" spans="1:3" ht="128.25" thickBot="1">
+      <c r="A10" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="29"/>
+    </row>
+    <row r="11" spans="1:3" ht="153.75" thickBot="1">
+      <c r="A11" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="29"/>
+    </row>
+    <row r="12" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A12" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="28"/>
+      <c r="C12" s="28"/>
+    </row>
+    <row r="13" spans="1:3" ht="77.25" thickBot="1">
+      <c r="A13" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="29" t="s">
+        <v>139</v>
+      </c>
+      <c r="C13" s="29"/>
+    </row>
+    <row r="14" spans="1:3" ht="64.5" thickBot="1">
+      <c r="A14" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="C14" s="29"/>
+    </row>
+    <row r="15" spans="1:3" ht="60.75" customHeight="1">
+      <c r="A15" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="25"/>
+    </row>
+    <row r="16" spans="1:3" ht="102" customHeight="1" thickBot="1">
+      <c r="A16" s="27"/>
+      <c r="B16" s="27" t="s">
+        <v>140</v>
+      </c>
+      <c r="C16" s="27"/>
+    </row>
+    <row r="17" spans="1:3" ht="26.25" thickBot="1">
+      <c r="A17" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="26.25" thickBot="1">
+      <c r="A18" s="26"/>
+      <c r="B18" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="51.75" thickBot="1">
+      <c r="A19" s="26"/>
+      <c r="B19" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="26.25" thickBot="1">
+      <c r="A20" s="26"/>
+      <c r="B20" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="26.25" thickBot="1">
+      <c r="A21" s="26"/>
+      <c r="B21" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="26.25" thickBot="1">
+      <c r="A22" s="26"/>
+      <c r="B22" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="26.25" thickBot="1">
+      <c r="A23" s="27"/>
+      <c r="B23" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="230.25" thickBot="1">
+      <c r="A24" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="29"/>
+      <c r="C24" s="29"/>
+    </row>
+    <row r="25" spans="1:3" ht="77.25" thickBot="1">
+      <c r="A25" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25" s="29"/>
+      <c r="C25" s="29"/>
+    </row>
+    <row r="26" spans="1:3" ht="64.5" thickBot="1">
+      <c r="A26" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" s="29"/>
+      <c r="C26" s="29"/>
+    </row>
+    <row r="27" spans="1:3" ht="141" thickBot="1">
+      <c r="A27" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="B27" s="29" t="s">
+        <v>100</v>
+      </c>
+      <c r="C27" s="29"/>
+    </row>
+    <row r="28" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A28" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="B28" s="28"/>
+      <c r="C28" s="28"/>
+    </row>
+    <row r="29" spans="1:3" ht="166.5" thickBot="1">
+      <c r="A29" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B29" s="29" t="s">
+        <v>141</v>
+      </c>
+      <c r="C29" s="29"/>
+    </row>
+    <row r="30" spans="1:3" ht="179.25" thickBot="1">
+      <c r="A30" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="B30" s="29" t="s">
+        <v>142</v>
+      </c>
+      <c r="C30" s="29"/>
+    </row>
+    <row r="31" spans="1:3" ht="77.25" thickBot="1">
+      <c r="A31" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="B31" s="29" t="s">
+        <v>142</v>
+      </c>
+      <c r="C31" s="29"/>
+    </row>
+    <row r="32" spans="1:3" ht="77.25" thickBot="1">
+      <c r="A32" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="77.25" thickBot="1">
+      <c r="A33" s="26"/>
+      <c r="B33" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="39" thickBot="1">
+      <c r="A34" s="26"/>
+      <c r="B34" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="26.25" thickBot="1">
+      <c r="A35" s="26"/>
+      <c r="B35" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="39" thickBot="1">
+      <c r="A36" s="26"/>
+      <c r="B36" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="39" thickBot="1">
+      <c r="A37" s="26"/>
+      <c r="B37" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="26.25" thickBot="1">
+      <c r="A38" s="26"/>
+      <c r="B38" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="26.25" thickBot="1">
+      <c r="A39" s="26"/>
+      <c r="B39" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="26.25" thickBot="1">
+      <c r="A40" s="26"/>
+      <c r="B40" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="51.75" thickBot="1">
+      <c r="A41" s="26"/>
+      <c r="B41" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="39" thickBot="1">
+      <c r="A42" s="26"/>
+      <c r="B42" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="26.25" thickBot="1">
+      <c r="A43" s="26"/>
+      <c r="B43" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="39" thickBot="1">
+      <c r="A44" s="26"/>
+      <c r="B44" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="77.25" thickBot="1">
+      <c r="A45" s="26"/>
+      <c r="B45" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="64.5" thickBot="1">
+      <c r="A46" s="26"/>
+      <c r="B46" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A47" s="26"/>
+      <c r="B47" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="26.25" thickBot="1">
+      <c r="A48" s="26"/>
+      <c r="B48" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A49" s="26"/>
+      <c r="B49" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="39" thickBot="1">
+      <c r="A50" s="26"/>
+      <c r="B50" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A51" s="26"/>
+      <c r="B51" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A52" s="26"/>
+      <c r="B52" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="115.5" thickBot="1">
+      <c r="A53" s="26"/>
+      <c r="B53" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="26.25" thickBot="1">
+      <c r="A54" s="26"/>
+      <c r="B54" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="77.25" thickBot="1">
+      <c r="A55" s="26"/>
+      <c r="B55" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A56" s="26"/>
+      <c r="B56" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="51.75" thickBot="1">
+      <c r="A57" s="26"/>
+      <c r="B57" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="77.25" thickBot="1">
+      <c r="A58" s="26"/>
+      <c r="B58" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="90" thickBot="1">
+      <c r="A59" s="26"/>
+      <c r="B59" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="77.25" thickBot="1">
+      <c r="A60" s="27"/>
+      <c r="B60" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A61" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="B61" s="28"/>
+      <c r="C61" s="28"/>
+    </row>
+    <row r="62" spans="1:3" ht="90" thickBot="1">
+      <c r="A62" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="B62" s="29"/>
+      <c r="C62" s="29"/>
+    </row>
+    <row r="63" spans="1:3" ht="64.5" thickBot="1">
+      <c r="A63" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="B63" s="29"/>
+      <c r="C63" s="29"/>
+    </row>
+    <row r="64" spans="1:3" ht="64.5" thickBot="1">
+      <c r="A64" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="B64" s="29"/>
+      <c r="C64" s="29"/>
+    </row>
+    <row r="65" spans="1:3" ht="51.75" thickBot="1">
+      <c r="A65" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="B65" s="29"/>
+      <c r="C65" s="29"/>
+    </row>
+    <row r="66" spans="1:3" ht="64.5" thickBot="1">
+      <c r="A66" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="B66" s="29"/>
+      <c r="C66" s="29"/>
+    </row>
+    <row r="67" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A67" s="28" t="s">
+        <v>85</v>
+      </c>
+      <c r="B67" s="28"/>
+      <c r="C67" s="28"/>
+    </row>
+    <row r="68" spans="1:3" ht="114.75" customHeight="1">
+      <c r="A68" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="B68" s="25" t="s">
+        <v>143</v>
+      </c>
+      <c r="C68" s="25"/>
+    </row>
+  </sheetData>
+  <mergeCells count="34">
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="A67:C67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="A32:A60"/>
+    <mergeCell ref="A61:C61"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="A17:A23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88791C71-46F4-4D83-BD43-DAD62B001B2F}">
   <dimension ref="A1:C67"/>
   <sheetViews>
@@ -2139,126 +2809,126 @@
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="18"/>
+      <c r="C2" s="30"/>
     </row>
     <row r="3" spans="1:3" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
     </row>
     <row r="4" spans="1:3" ht="26.25" thickBot="1">
       <c r="A4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="17"/>
+      <c r="C4" s="29"/>
     </row>
     <row r="5" spans="1:3" ht="39" thickBot="1">
       <c r="A5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="17"/>
+      <c r="C5" s="29"/>
     </row>
     <row r="6" spans="1:3" ht="15.75" thickBot="1">
       <c r="A6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="29" t="s">
         <v>96</v>
       </c>
-      <c r="C6" s="17"/>
+      <c r="C6" s="29"/>
     </row>
     <row r="7" spans="1:3" ht="39" thickBot="1">
       <c r="A7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="17">
+      <c r="B7" s="29">
         <v>1</v>
       </c>
-      <c r="C7" s="17"/>
+      <c r="C7" s="29"/>
     </row>
     <row r="8" spans="1:3" ht="26.25" thickBot="1">
       <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="17">
+      <c r="B8" s="29">
         <v>2</v>
       </c>
-      <c r="C8" s="17"/>
+      <c r="C8" s="29"/>
     </row>
     <row r="9" spans="1:3" ht="26.25" thickBot="1">
       <c r="A9" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="17">
+      <c r="B9" s="29">
         <v>2</v>
       </c>
-      <c r="C9" s="17"/>
+      <c r="C9" s="29"/>
     </row>
     <row r="10" spans="1:3" ht="26.25" thickBot="1">
       <c r="A10" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="17"/>
+      <c r="C10" s="29"/>
     </row>
     <row r="11" spans="1:3" ht="26.25" thickBot="1">
       <c r="A11" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="29" t="s">
         <v>97</v>
       </c>
-      <c r="C11" s="17"/>
+      <c r="C11" s="29"/>
     </row>
     <row r="12" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A12" s="22" t="s">
+      <c r="A12" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="22"/>
-      <c r="C12" s="22"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="28"/>
     </row>
     <row r="13" spans="1:3" ht="15.75" thickBot="1">
       <c r="A13" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="17">
+      <c r="B13" s="29">
         <v>10</v>
       </c>
-      <c r="C13" s="17"/>
+      <c r="C13" s="29"/>
     </row>
     <row r="14" spans="1:3" ht="15.75" thickBot="1">
       <c r="A14" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="C14" s="17"/>
+      <c r="C14" s="29"/>
     </row>
     <row r="15" spans="1:3" ht="15.75" thickBot="1">
       <c r="A15" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="C15" s="17"/>
+      <c r="C15" s="29"/>
     </row>
     <row r="16" spans="1:3" ht="29.25" customHeight="1" thickBot="1">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="25" t="s">
         <v>26</v>
       </c>
       <c r="B16" s="4" t="s">
@@ -2269,7 +2939,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A17" s="23"/>
+      <c r="A17" s="26"/>
       <c r="B17" s="4" t="s">
         <v>29</v>
       </c>
@@ -2278,7 +2948,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" ht="26.25" thickBot="1">
-      <c r="A18" s="23"/>
+      <c r="A18" s="26"/>
       <c r="B18" s="4" t="s">
         <v>31</v>
       </c>
@@ -2287,7 +2957,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A19" s="23"/>
+      <c r="A19" s="26"/>
       <c r="B19" s="4" t="s">
         <v>33</v>
       </c>
@@ -2296,7 +2966,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A20" s="23"/>
+      <c r="A20" s="26"/>
       <c r="B20" s="4" t="s">
         <v>34</v>
       </c>
@@ -2305,7 +2975,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A21" s="23"/>
+      <c r="A21" s="26"/>
       <c r="B21" s="4" t="s">
         <v>35</v>
       </c>
@@ -2314,7 +2984,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A22" s="21"/>
+      <c r="A22" s="27"/>
       <c r="B22" s="4" t="s">
         <v>36</v>
       </c>
@@ -2326,68 +2996,68 @@
       <c r="A23" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="17"/>
-      <c r="C23" s="17"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="29"/>
     </row>
     <row r="24" spans="1:3" ht="15.75" thickBot="1">
       <c r="A24" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B24" s="17"/>
-      <c r="C24" s="17"/>
+      <c r="B24" s="29"/>
+      <c r="C24" s="29"/>
     </row>
     <row r="25" spans="1:3" ht="15.75" thickBot="1">
       <c r="A25" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B25" s="17"/>
-      <c r="C25" s="17"/>
+      <c r="B25" s="29"/>
+      <c r="C25" s="29"/>
     </row>
     <row r="26" spans="1:3" ht="26.25" thickBot="1">
       <c r="A26" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="29" t="s">
         <v>100</v>
       </c>
-      <c r="C26" s="17"/>
+      <c r="C26" s="29"/>
     </row>
     <row r="27" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A27" s="22" t="s">
+      <c r="A27" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="B27" s="22"/>
-      <c r="C27" s="22"/>
+      <c r="B27" s="28"/>
+      <c r="C27" s="28"/>
     </row>
     <row r="28" spans="1:3" ht="39" thickBot="1">
       <c r="A28" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B28" s="17" t="s">
+      <c r="B28" s="29" t="s">
         <v>101</v>
       </c>
-      <c r="C28" s="17"/>
+      <c r="C28" s="29"/>
     </row>
     <row r="29" spans="1:3" ht="39" thickBot="1">
       <c r="A29" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B29" s="17" t="s">
+      <c r="B29" s="29" t="s">
         <v>102</v>
       </c>
-      <c r="C29" s="17"/>
+      <c r="C29" s="29"/>
     </row>
     <row r="30" spans="1:3" ht="15.75" thickBot="1">
       <c r="A30" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B30" s="17" t="s">
+      <c r="B30" s="29" t="s">
         <v>103</v>
       </c>
-      <c r="C30" s="17"/>
+      <c r="C30" s="29"/>
     </row>
     <row r="31" spans="1:3" ht="39" thickBot="1">
-      <c r="A31" s="20" t="s">
+      <c r="A31" s="25" t="s">
         <v>49</v>
       </c>
       <c r="B31" s="4" t="s">
@@ -2396,261 +3066,281 @@
       <c r="C31" s="5"/>
     </row>
     <row r="32" spans="1:3" ht="39" thickBot="1">
-      <c r="A32" s="23"/>
+      <c r="A32" s="26"/>
       <c r="B32" s="4" t="s">
         <v>51</v>
       </c>
       <c r="C32" s="5"/>
     </row>
     <row r="33" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A33" s="23"/>
+      <c r="A33" s="26"/>
       <c r="B33" s="4" t="s">
         <v>52</v>
       </c>
       <c r="C33" s="5"/>
     </row>
     <row r="34" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A34" s="23"/>
+      <c r="A34" s="26"/>
       <c r="B34" s="4" t="s">
         <v>53</v>
       </c>
       <c r="C34" s="5"/>
     </row>
     <row r="35" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A35" s="23"/>
+      <c r="A35" s="26"/>
       <c r="B35" s="4" t="s">
         <v>54</v>
       </c>
       <c r="C35" s="5"/>
     </row>
     <row r="36" spans="1:3" ht="26.25" thickBot="1">
-      <c r="A36" s="23"/>
+      <c r="A36" s="26"/>
       <c r="B36" s="4" t="s">
         <v>55</v>
       </c>
       <c r="C36" s="5"/>
     </row>
     <row r="37" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A37" s="23"/>
+      <c r="A37" s="26"/>
       <c r="B37" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C37" s="5"/>
     </row>
     <row r="38" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A38" s="23"/>
+      <c r="A38" s="26"/>
       <c r="B38" s="4" t="s">
         <v>57</v>
       </c>
       <c r="C38" s="5"/>
     </row>
     <row r="39" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A39" s="23"/>
+      <c r="A39" s="26"/>
       <c r="B39" s="4" t="s">
         <v>58</v>
       </c>
       <c r="C39" s="5"/>
     </row>
     <row r="40" spans="1:3" ht="26.25" thickBot="1">
-      <c r="A40" s="23"/>
+      <c r="A40" s="26"/>
       <c r="B40" s="4" t="s">
         <v>59</v>
       </c>
       <c r="C40" s="5"/>
     </row>
     <row r="41" spans="1:3" ht="26.25" thickBot="1">
-      <c r="A41" s="23"/>
+      <c r="A41" s="26"/>
       <c r="B41" s="4" t="s">
         <v>60</v>
       </c>
       <c r="C41" s="5"/>
     </row>
     <row r="42" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A42" s="23"/>
+      <c r="A42" s="26"/>
       <c r="B42" s="4" t="s">
         <v>61</v>
       </c>
       <c r="C42" s="5"/>
     </row>
     <row r="43" spans="1:3" ht="26.25" thickBot="1">
-      <c r="A43" s="23"/>
+      <c r="A43" s="26"/>
       <c r="B43" s="4" t="s">
         <v>62</v>
       </c>
       <c r="C43" s="5"/>
     </row>
     <row r="44" spans="1:3" ht="39" thickBot="1">
-      <c r="A44" s="23"/>
+      <c r="A44" s="26"/>
       <c r="B44" s="4" t="s">
         <v>63</v>
       </c>
       <c r="C44" s="5"/>
     </row>
     <row r="45" spans="1:3" ht="39" thickBot="1">
-      <c r="A45" s="23"/>
+      <c r="A45" s="26"/>
       <c r="B45" s="4" t="s">
         <v>64</v>
       </c>
       <c r="C45" s="5"/>
     </row>
     <row r="46" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A46" s="23"/>
+      <c r="A46" s="26"/>
       <c r="B46" s="4" t="s">
         <v>65</v>
       </c>
       <c r="C46" s="5"/>
     </row>
     <row r="47" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A47" s="23"/>
+      <c r="A47" s="26"/>
       <c r="B47" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C47" s="5"/>
     </row>
     <row r="48" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A48" s="23"/>
+      <c r="A48" s="26"/>
       <c r="B48" s="4" t="s">
         <v>67</v>
       </c>
       <c r="C48" s="5"/>
     </row>
     <row r="49" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A49" s="23"/>
+      <c r="A49" s="26"/>
       <c r="B49" s="4" t="s">
         <v>68</v>
       </c>
       <c r="C49" s="5"/>
     </row>
     <row r="50" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A50" s="23"/>
+      <c r="A50" s="26"/>
       <c r="B50" s="4" t="s">
         <v>69</v>
       </c>
       <c r="C50" s="5"/>
     </row>
     <row r="51" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A51" s="23"/>
+      <c r="A51" s="26"/>
       <c r="B51" s="4" t="s">
         <v>70</v>
       </c>
       <c r="C51" s="5"/>
     </row>
     <row r="52" spans="1:3" ht="51.75" thickBot="1">
-      <c r="A52" s="23"/>
+      <c r="A52" s="26"/>
       <c r="B52" s="4" t="s">
         <v>71</v>
       </c>
       <c r="C52" s="5"/>
     </row>
     <row r="53" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A53" s="23"/>
+      <c r="A53" s="26"/>
       <c r="B53" s="4" t="s">
         <v>72</v>
       </c>
       <c r="C53" s="5"/>
     </row>
     <row r="54" spans="1:3" ht="39" thickBot="1">
-      <c r="A54" s="23"/>
+      <c r="A54" s="26"/>
       <c r="B54" s="4" t="s">
         <v>73</v>
       </c>
       <c r="C54" s="5"/>
     </row>
     <row r="55" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A55" s="23"/>
+      <c r="A55" s="26"/>
       <c r="B55" s="4" t="s">
         <v>74</v>
       </c>
       <c r="C55" s="5"/>
     </row>
     <row r="56" spans="1:3" ht="26.25" thickBot="1">
-      <c r="A56" s="23"/>
+      <c r="A56" s="26"/>
       <c r="B56" s="4" t="s">
         <v>75</v>
       </c>
       <c r="C56" s="5"/>
     </row>
     <row r="57" spans="1:3" ht="39" thickBot="1">
-      <c r="A57" s="23"/>
+      <c r="A57" s="26"/>
       <c r="B57" s="4" t="s">
         <v>76</v>
       </c>
       <c r="C57" s="5"/>
     </row>
     <row r="58" spans="1:3" ht="39" thickBot="1">
-      <c r="A58" s="23"/>
+      <c r="A58" s="26"/>
       <c r="B58" s="4" t="s">
         <v>77</v>
       </c>
       <c r="C58" s="5"/>
     </row>
     <row r="59" spans="1:3" ht="39" thickBot="1">
-      <c r="A59" s="21"/>
+      <c r="A59" s="27"/>
       <c r="B59" s="4" t="s">
         <v>78</v>
       </c>
       <c r="C59" s="5"/>
     </row>
     <row r="60" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A60" s="22" t="s">
+      <c r="A60" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="B60" s="22"/>
-      <c r="C60" s="22"/>
+      <c r="B60" s="28"/>
+      <c r="C60" s="28"/>
     </row>
     <row r="61" spans="1:3" ht="26.25" thickBot="1">
       <c r="A61" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="B61" s="17"/>
-      <c r="C61" s="17"/>
+      <c r="B61" s="29"/>
+      <c r="C61" s="29"/>
     </row>
     <row r="62" spans="1:3" ht="15.75" thickBot="1">
       <c r="A62" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="B62" s="17"/>
-      <c r="C62" s="17"/>
+      <c r="B62" s="29"/>
+      <c r="C62" s="29"/>
     </row>
     <row r="63" spans="1:3" ht="15.75" thickBot="1">
       <c r="A63" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="B63" s="17"/>
-      <c r="C63" s="17"/>
+      <c r="B63" s="29"/>
+      <c r="C63" s="29"/>
     </row>
     <row r="64" spans="1:3" ht="15.75" thickBot="1">
       <c r="A64" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="B64" s="17"/>
-      <c r="C64" s="17"/>
+      <c r="B64" s="29"/>
+      <c r="C64" s="29"/>
     </row>
     <row r="65" spans="1:3" ht="15.75" thickBot="1">
       <c r="A65" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="B65" s="17"/>
-      <c r="C65" s="17"/>
+      <c r="B65" s="29"/>
+      <c r="C65" s="29"/>
     </row>
     <row r="66" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A66" s="22" t="s">
+      <c r="A66" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="B66" s="22"/>
-      <c r="C66" s="22"/>
+      <c r="B66" s="28"/>
+      <c r="C66" s="28"/>
     </row>
     <row r="67" spans="1:3" ht="25.5">
       <c r="A67" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="B67" s="20" t="s">
+      <c r="B67" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="C67" s="20"/>
+      <c r="C67" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="A66:C66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="A60:C60"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="A31:A59"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="A16:A22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="A3:C3"/>
@@ -2663,26 +3353,6 @@
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A31:A59"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="A16:A22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="A66:C66"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="A60:C60"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B65:C65"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -2690,7 +3360,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A370E2B2-1D66-4FCA-82A6-A01DA52CD0E0}">
   <dimension ref="A29:C97"/>
   <sheetViews>
@@ -2712,140 +3382,140 @@
       <c r="A30" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B30" s="30" t="s">
+      <c r="B30" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="C30" s="30"/>
+      <c r="C30" s="32"/>
     </row>
     <row r="31" spans="1:3" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A31" s="31" t="s">
+      <c r="A31" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="B31" s="31"/>
-      <c r="C31" s="31"/>
+      <c r="B31" s="33"/>
+      <c r="C31" s="33"/>
     </row>
     <row r="32" spans="1:3" ht="26.25" thickBot="1">
       <c r="A32" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B32" s="24" t="s">
+      <c r="B32" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="C32" s="24"/>
+      <c r="C32" s="34"/>
     </row>
     <row r="33" spans="1:3" ht="39" thickBot="1">
       <c r="A33" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="B33" s="24" t="s">
+      <c r="B33" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="C33" s="24"/>
+      <c r="C33" s="34"/>
     </row>
     <row r="34" spans="1:3" ht="48" customHeight="1">
-      <c r="A34" s="26" t="s">
+      <c r="A34" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="B34" s="26" t="s">
+      <c r="B34" s="35" t="s">
         <v>106</v>
       </c>
-      <c r="C34" s="26"/>
+      <c r="C34" s="35"/>
     </row>
     <row r="35" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A35" s="28"/>
-      <c r="B35" s="28" t="s">
+      <c r="A35" s="36"/>
+      <c r="B35" s="36" t="s">
         <v>107</v>
       </c>
-      <c r="C35" s="28"/>
+      <c r="C35" s="36"/>
     </row>
     <row r="36" spans="1:3" ht="51.75" thickBot="1">
       <c r="A36" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B36" s="24">
+      <c r="B36" s="34">
         <v>1</v>
       </c>
-      <c r="C36" s="24"/>
+      <c r="C36" s="34"/>
     </row>
     <row r="37" spans="1:3" ht="39" thickBot="1">
       <c r="A37" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B37" s="24">
+      <c r="B37" s="34">
         <v>1</v>
       </c>
-      <c r="C37" s="24"/>
+      <c r="C37" s="34"/>
     </row>
     <row r="38" spans="1:3" ht="39" thickBot="1">
       <c r="A38" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B38" s="24">
+      <c r="B38" s="34">
         <v>1</v>
       </c>
-      <c r="C38" s="24"/>
+      <c r="C38" s="34"/>
     </row>
     <row r="39" spans="1:3" ht="26.25" thickBot="1">
       <c r="A39" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B39" s="24" t="s">
+      <c r="B39" s="34" t="s">
         <v>108</v>
       </c>
-      <c r="C39" s="24"/>
+      <c r="C39" s="34"/>
     </row>
     <row r="40" spans="1:3" ht="137.25" customHeight="1">
-      <c r="A40" s="26" t="s">
+      <c r="A40" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="B40" s="26" t="s">
+      <c r="B40" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="C40" s="26"/>
+      <c r="C40" s="35"/>
     </row>
     <row r="41" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A41" s="28"/>
-      <c r="B41" s="28" t="s">
+      <c r="A41" s="36"/>
+      <c r="B41" s="36" t="s">
         <v>109</v>
       </c>
-      <c r="C41" s="28"/>
+      <c r="C41" s="36"/>
     </row>
     <row r="42" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A42" s="29" t="s">
+      <c r="A42" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="B42" s="29"/>
-      <c r="C42" s="29"/>
+      <c r="B42" s="37"/>
+      <c r="C42" s="37"/>
     </row>
     <row r="43" spans="1:3" ht="15.75" thickBot="1">
       <c r="A43" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B43" s="24" t="s">
+      <c r="B43" s="34" t="s">
         <v>110</v>
       </c>
-      <c r="C43" s="24"/>
+      <c r="C43" s="34"/>
     </row>
     <row r="44" spans="1:3" ht="15.75" thickBot="1">
       <c r="A44" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="B44" s="24" t="s">
+      <c r="B44" s="34" t="s">
         <v>111</v>
       </c>
-      <c r="C44" s="24"/>
+      <c r="C44" s="34"/>
     </row>
     <row r="45" spans="1:3" ht="15.75" thickBot="1">
       <c r="A45" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B45" s="24" t="s">
+      <c r="B45" s="34" t="s">
         <v>99</v>
       </c>
-      <c r="C45" s="24"/>
+      <c r="C45" s="34"/>
     </row>
     <row r="46" spans="1:3" ht="29.25" customHeight="1" thickBot="1">
-      <c r="A46" s="26" t="s">
+      <c r="A46" s="35" t="s">
         <v>26</v>
       </c>
       <c r="B46" s="4" t="s">
@@ -2856,7 +3526,7 @@
       </c>
     </row>
     <row r="47" spans="1:3" ht="26.25" thickBot="1">
-      <c r="A47" s="27"/>
+      <c r="A47" s="38"/>
       <c r="B47" s="4" t="s">
         <v>29</v>
       </c>
@@ -2865,7 +3535,7 @@
       </c>
     </row>
     <row r="48" spans="1:3" ht="51.75" thickBot="1">
-      <c r="A48" s="27"/>
+      <c r="A48" s="38"/>
       <c r="B48" s="4" t="s">
         <v>31</v>
       </c>
@@ -2874,7 +3544,7 @@
       </c>
     </row>
     <row r="49" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A49" s="27"/>
+      <c r="A49" s="38"/>
       <c r="B49" s="4" t="s">
         <v>33</v>
       </c>
@@ -2883,7 +3553,7 @@
       </c>
     </row>
     <row r="50" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A50" s="27"/>
+      <c r="A50" s="38"/>
       <c r="B50" s="4" t="s">
         <v>34</v>
       </c>
@@ -2892,7 +3562,7 @@
       </c>
     </row>
     <row r="51" spans="1:3" ht="26.25" thickBot="1">
-      <c r="A51" s="27"/>
+      <c r="A51" s="38"/>
       <c r="B51" s="4" t="s">
         <v>35</v>
       </c>
@@ -2901,7 +3571,7 @@
       </c>
     </row>
     <row r="52" spans="1:3" ht="26.25" thickBot="1">
-      <c r="A52" s="28"/>
+      <c r="A52" s="36"/>
       <c r="B52" s="4" t="s">
         <v>36</v>
       </c>
@@ -2913,64 +3583,64 @@
       <c r="A53" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="B53" s="24"/>
-      <c r="C53" s="24"/>
+      <c r="B53" s="34"/>
+      <c r="C53" s="34"/>
     </row>
     <row r="54" spans="1:3" ht="15.75" thickBot="1">
       <c r="A54" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="B54" s="24"/>
-      <c r="C54" s="24"/>
+      <c r="B54" s="34"/>
+      <c r="C54" s="34"/>
     </row>
     <row r="55" spans="1:3" ht="15.75" thickBot="1">
       <c r="A55" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="B55" s="24"/>
-      <c r="C55" s="24"/>
+      <c r="B55" s="34"/>
+      <c r="C55" s="34"/>
     </row>
     <row r="56" spans="1:3" ht="39" thickBot="1">
       <c r="A56" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="B56" s="24" t="s">
+      <c r="B56" s="34" t="s">
         <v>100</v>
       </c>
-      <c r="C56" s="24"/>
+      <c r="C56" s="34"/>
     </row>
     <row r="57" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A57" s="29" t="s">
+      <c r="A57" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="B57" s="29"/>
-      <c r="C57" s="29"/>
+      <c r="B57" s="37"/>
+      <c r="C57" s="37"/>
     </row>
     <row r="58" spans="1:3" ht="39" thickBot="1">
       <c r="A58" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="B58" s="24" t="s">
+      <c r="B58" s="34" t="s">
         <v>112</v>
       </c>
-      <c r="C58" s="24"/>
+      <c r="C58" s="34"/>
     </row>
     <row r="59" spans="1:3" ht="39" thickBot="1">
       <c r="A59" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="B59" s="24"/>
-      <c r="C59" s="24"/>
+      <c r="B59" s="34"/>
+      <c r="C59" s="34"/>
     </row>
     <row r="60" spans="1:3" ht="26.25" thickBot="1">
       <c r="A60" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="B60" s="24"/>
-      <c r="C60" s="24"/>
+      <c r="B60" s="34"/>
+      <c r="C60" s="34"/>
     </row>
     <row r="61" spans="1:3" ht="77.25" thickBot="1">
-      <c r="A61" s="26" t="s">
+      <c r="A61" s="35" t="s">
         <v>49</v>
       </c>
       <c r="B61" s="4" t="s">
@@ -2979,249 +3649,249 @@
       <c r="C61" s="5"/>
     </row>
     <row r="62" spans="1:3" ht="77.25" thickBot="1">
-      <c r="A62" s="27"/>
+      <c r="A62" s="38"/>
       <c r="B62" s="4" t="s">
         <v>51</v>
       </c>
       <c r="C62" s="5"/>
     </row>
     <row r="63" spans="1:3" ht="39" thickBot="1">
-      <c r="A63" s="27"/>
+      <c r="A63" s="38"/>
       <c r="B63" s="4" t="s">
         <v>52</v>
       </c>
       <c r="C63" s="5"/>
     </row>
     <row r="64" spans="1:3" ht="26.25" thickBot="1">
-      <c r="A64" s="27"/>
+      <c r="A64" s="38"/>
       <c r="B64" s="4" t="s">
         <v>53</v>
       </c>
       <c r="C64" s="5"/>
     </row>
     <row r="65" spans="1:3" ht="39" thickBot="1">
-      <c r="A65" s="27"/>
+      <c r="A65" s="38"/>
       <c r="B65" s="4" t="s">
         <v>54</v>
       </c>
       <c r="C65" s="5"/>
     </row>
     <row r="66" spans="1:3" ht="39" thickBot="1">
-      <c r="A66" s="27"/>
+      <c r="A66" s="38"/>
       <c r="B66" s="4" t="s">
         <v>55</v>
       </c>
       <c r="C66" s="5"/>
     </row>
     <row r="67" spans="1:3" ht="26.25" thickBot="1">
-      <c r="A67" s="27"/>
+      <c r="A67" s="38"/>
       <c r="B67" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C67" s="5"/>
     </row>
     <row r="68" spans="1:3" ht="26.25" thickBot="1">
-      <c r="A68" s="27"/>
+      <c r="A68" s="38"/>
       <c r="B68" s="4" t="s">
         <v>57</v>
       </c>
       <c r="C68" s="5"/>
     </row>
     <row r="69" spans="1:3" ht="26.25" thickBot="1">
-      <c r="A69" s="27"/>
+      <c r="A69" s="38"/>
       <c r="B69" s="4" t="s">
         <v>58</v>
       </c>
       <c r="C69" s="5"/>
     </row>
     <row r="70" spans="1:3" ht="51.75" thickBot="1">
-      <c r="A70" s="27"/>
+      <c r="A70" s="38"/>
       <c r="B70" s="4" t="s">
         <v>59</v>
       </c>
       <c r="C70" s="5"/>
     </row>
     <row r="71" spans="1:3" ht="39" thickBot="1">
-      <c r="A71" s="27"/>
+      <c r="A71" s="38"/>
       <c r="B71" s="4" t="s">
         <v>60</v>
       </c>
       <c r="C71" s="5"/>
     </row>
     <row r="72" spans="1:3" ht="26.25" thickBot="1">
-      <c r="A72" s="27"/>
+      <c r="A72" s="38"/>
       <c r="B72" s="4" t="s">
         <v>61</v>
       </c>
       <c r="C72" s="5"/>
     </row>
     <row r="73" spans="1:3" ht="39" thickBot="1">
-      <c r="A73" s="27"/>
+      <c r="A73" s="38"/>
       <c r="B73" s="4" t="s">
         <v>62</v>
       </c>
       <c r="C73" s="5"/>
     </row>
     <row r="74" spans="1:3" ht="77.25" thickBot="1">
-      <c r="A74" s="27"/>
+      <c r="A74" s="38"/>
       <c r="B74" s="4" t="s">
         <v>63</v>
       </c>
       <c r="C74" s="5"/>
     </row>
     <row r="75" spans="1:3" ht="64.5" thickBot="1">
-      <c r="A75" s="27"/>
+      <c r="A75" s="38"/>
       <c r="B75" s="4" t="s">
         <v>64</v>
       </c>
       <c r="C75" s="5"/>
     </row>
     <row r="76" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A76" s="27"/>
+      <c r="A76" s="38"/>
       <c r="B76" s="4" t="s">
         <v>65</v>
       </c>
       <c r="C76" s="5"/>
     </row>
     <row r="77" spans="1:3" ht="26.25" thickBot="1">
-      <c r="A77" s="27"/>
+      <c r="A77" s="38"/>
       <c r="B77" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C77" s="5"/>
     </row>
     <row r="78" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A78" s="27"/>
+      <c r="A78" s="38"/>
       <c r="B78" s="4" t="s">
         <v>67</v>
       </c>
       <c r="C78" s="5"/>
     </row>
     <row r="79" spans="1:3" ht="39" thickBot="1">
-      <c r="A79" s="27"/>
+      <c r="A79" s="38"/>
       <c r="B79" s="4" t="s">
         <v>68</v>
       </c>
       <c r="C79" s="5"/>
     </row>
     <row r="80" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A80" s="27"/>
+      <c r="A80" s="38"/>
       <c r="B80" s="4" t="s">
         <v>69</v>
       </c>
       <c r="C80" s="5"/>
     </row>
     <row r="81" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A81" s="27"/>
+      <c r="A81" s="38"/>
       <c r="B81" s="4" t="s">
         <v>70</v>
       </c>
       <c r="C81" s="5"/>
     </row>
     <row r="82" spans="1:3" ht="115.5" thickBot="1">
-      <c r="A82" s="27"/>
+      <c r="A82" s="38"/>
       <c r="B82" s="4" t="s">
         <v>71</v>
       </c>
       <c r="C82" s="5"/>
     </row>
     <row r="83" spans="1:3" ht="26.25" thickBot="1">
-      <c r="A83" s="27"/>
+      <c r="A83" s="38"/>
       <c r="B83" s="4" t="s">
         <v>72</v>
       </c>
       <c r="C83" s="5"/>
     </row>
     <row r="84" spans="1:3" ht="77.25" thickBot="1">
-      <c r="A84" s="27"/>
+      <c r="A84" s="38"/>
       <c r="B84" s="4" t="s">
         <v>73</v>
       </c>
       <c r="C84" s="5"/>
     </row>
     <row r="85" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A85" s="27"/>
+      <c r="A85" s="38"/>
       <c r="B85" s="4" t="s">
         <v>74</v>
       </c>
       <c r="C85" s="5"/>
     </row>
     <row r="86" spans="1:3" ht="51.75" thickBot="1">
-      <c r="A86" s="27"/>
+      <c r="A86" s="38"/>
       <c r="B86" s="4" t="s">
         <v>75</v>
       </c>
       <c r="C86" s="5"/>
     </row>
     <row r="87" spans="1:3" ht="77.25" thickBot="1">
-      <c r="A87" s="27"/>
+      <c r="A87" s="38"/>
       <c r="B87" s="4" t="s">
         <v>76</v>
       </c>
       <c r="C87" s="5"/>
     </row>
     <row r="88" spans="1:3" ht="90" thickBot="1">
-      <c r="A88" s="27"/>
+      <c r="A88" s="38"/>
       <c r="B88" s="4" t="s">
         <v>77</v>
       </c>
       <c r="C88" s="5"/>
     </row>
     <row r="89" spans="1:3" ht="77.25" thickBot="1">
-      <c r="A89" s="28"/>
+      <c r="A89" s="36"/>
       <c r="B89" s="4" t="s">
         <v>78</v>
       </c>
       <c r="C89" s="5"/>
     </row>
     <row r="90" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A90" s="29" t="s">
+      <c r="A90" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="B90" s="29"/>
-      <c r="C90" s="29"/>
+      <c r="B90" s="37"/>
+      <c r="C90" s="37"/>
     </row>
     <row r="91" spans="1:3" ht="26.25" thickBot="1">
       <c r="A91" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="B91" s="24"/>
-      <c r="C91" s="24"/>
+      <c r="B91" s="34"/>
+      <c r="C91" s="34"/>
     </row>
     <row r="92" spans="1:3" ht="15.75" thickBot="1">
       <c r="A92" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="B92" s="24"/>
-      <c r="C92" s="24"/>
+      <c r="B92" s="34"/>
+      <c r="C92" s="34"/>
     </row>
     <row r="93" spans="1:3" ht="15.75" thickBot="1">
       <c r="A93" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="B93" s="24"/>
-      <c r="C93" s="24"/>
+      <c r="B93" s="34"/>
+      <c r="C93" s="34"/>
     </row>
     <row r="94" spans="1:3" ht="15.75" thickBot="1">
       <c r="A94" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="B94" s="24"/>
-      <c r="C94" s="24"/>
+      <c r="B94" s="34"/>
+      <c r="C94" s="34"/>
     </row>
     <row r="95" spans="1:3" ht="15.75" thickBot="1">
       <c r="A95" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="B95" s="24"/>
-      <c r="C95" s="24"/>
+      <c r="B95" s="34"/>
+      <c r="C95" s="34"/>
     </row>
     <row r="96" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A96" s="25" t="s">
+      <c r="A96" s="39" t="s">
         <v>85</v>
       </c>
-      <c r="B96" s="25"/>
-      <c r="C96" s="25"/>
+      <c r="B96" s="39"/>
+      <c r="C96" s="39"/>
     </row>
     <row r="97" spans="1:1" ht="28.5">
       <c r="A97" s="16" t="s">
@@ -3230,20 +3900,15 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="A40:A41"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B94:C94"/>
+    <mergeCell ref="B95:C95"/>
+    <mergeCell ref="A96:C96"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="A61:A89"/>
+    <mergeCell ref="A90:C90"/>
+    <mergeCell ref="B91:C91"/>
+    <mergeCell ref="B92:C92"/>
+    <mergeCell ref="B93:C93"/>
     <mergeCell ref="B59:C59"/>
     <mergeCell ref="A42:C42"/>
     <mergeCell ref="B43:C43"/>
@@ -3256,15 +3921,20 @@
     <mergeCell ref="B56:C56"/>
     <mergeCell ref="A57:C57"/>
     <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B94:C94"/>
-    <mergeCell ref="B95:C95"/>
-    <mergeCell ref="A96:C96"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="A61:A89"/>
-    <mergeCell ref="A90:C90"/>
-    <mergeCell ref="B91:C91"/>
-    <mergeCell ref="B92:C92"/>
-    <mergeCell ref="B93:C93"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -3272,7 +3942,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22B90795-4172-4ABD-A79D-8943F4857E6F}">
   <dimension ref="A1:C67"/>
   <sheetViews>
@@ -3286,137 +3956,137 @@
     <col min="2" max="2" width="22.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="27" thickBot="1">
-      <c r="A1" s="33" t="s">
+    <row r="1" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="35"/>
+      <c r="C1" s="46"/>
     </row>
     <row r="2" spans="1:3" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-    </row>
-    <row r="3" spans="1:3" ht="115.5" thickBot="1">
-      <c r="A3" s="34" t="s">
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+    </row>
+    <row r="3" spans="1:3" ht="26.25" thickBot="1">
+      <c r="A3" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="40" t="s">
         <v>113</v>
       </c>
-      <c r="C3" s="39"/>
-    </row>
-    <row r="4" spans="1:3" ht="166.5" thickBot="1">
-      <c r="A4" s="34" t="s">
+      <c r="C3" s="40"/>
+    </row>
+    <row r="4" spans="1:3" ht="39" thickBot="1">
+      <c r="A4" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="39"/>
+      <c r="C4" s="40"/>
     </row>
     <row r="5" spans="1:3" ht="48" customHeight="1">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="38" t="s">
+      <c r="B5" s="42" t="s">
         <v>96</v>
       </c>
-      <c r="C5" s="38"/>
+      <c r="C5" s="42"/>
     </row>
     <row r="6" spans="1:3" ht="51" customHeight="1" thickBot="1">
-      <c r="A6" s="40"/>
-      <c r="B6" s="40" t="s">
+      <c r="A6" s="44"/>
+      <c r="B6" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="40"/>
-    </row>
-    <row r="7" spans="1:3" ht="230.25" thickBot="1">
-      <c r="A7" s="34" t="s">
+      <c r="C6" s="44"/>
+    </row>
+    <row r="7" spans="1:3" ht="39" thickBot="1">
+      <c r="A7" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="39">
+      <c r="B7" s="40">
         <v>5</v>
       </c>
-      <c r="C7" s="39"/>
-    </row>
-    <row r="8" spans="1:3" ht="115.5" thickBot="1">
-      <c r="A8" s="34" t="s">
+      <c r="C7" s="40"/>
+    </row>
+    <row r="8" spans="1:3" ht="26.25" thickBot="1">
+      <c r="A8" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="39">
+      <c r="B8" s="40">
         <v>3</v>
       </c>
-      <c r="C8" s="39"/>
-    </row>
-    <row r="9" spans="1:3" ht="141" thickBot="1">
-      <c r="A9" s="34" t="s">
+      <c r="C8" s="40"/>
+    </row>
+    <row r="9" spans="1:3" ht="26.25" thickBot="1">
+      <c r="A9" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="39">
+      <c r="B9" s="40">
         <v>3</v>
       </c>
-      <c r="C9" s="39"/>
-    </row>
-    <row r="10" spans="1:3" ht="128.25" thickBot="1">
-      <c r="A10" s="34" t="s">
+      <c r="C9" s="40"/>
+    </row>
+    <row r="10" spans="1:3" ht="26.25" thickBot="1">
+      <c r="A10" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="39" t="s">
+      <c r="B10" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="39"/>
-    </row>
-    <row r="11" spans="1:3" ht="153.75" thickBot="1">
-      <c r="A11" s="34" t="s">
+      <c r="C10" s="40"/>
+    </row>
+    <row r="11" spans="1:3" ht="26.25" thickBot="1">
+      <c r="A11" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="39" t="s">
+      <c r="B11" s="40" t="s">
         <v>97</v>
       </c>
-      <c r="C11" s="39"/>
+      <c r="C11" s="40"/>
     </row>
     <row r="12" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A12" s="41" t="s">
+      <c r="A12" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="41"/>
-      <c r="C12" s="41"/>
-    </row>
-    <row r="13" spans="1:3" ht="77.25" thickBot="1">
-      <c r="A13" s="34" t="s">
+      <c r="B12" s="45"/>
+      <c r="C12" s="45"/>
+    </row>
+    <row r="13" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A13" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="39" t="s">
+      <c r="B13" s="40" t="s">
         <v>114</v>
       </c>
-      <c r="C13" s="39"/>
-    </row>
-    <row r="14" spans="1:3" ht="64.5" thickBot="1">
-      <c r="A14" s="34" t="s">
+      <c r="C13" s="40"/>
+    </row>
+    <row r="14" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A14" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="39" t="s">
+      <c r="B14" s="40" t="s">
         <v>115</v>
       </c>
-      <c r="C14" s="39"/>
-    </row>
-    <row r="15" spans="1:3" ht="77.25" thickBot="1">
-      <c r="A15" s="34" t="s">
+      <c r="C14" s="40"/>
+    </row>
+    <row r="15" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A15" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="39" t="s">
+      <c r="B15" s="40" t="s">
         <v>99</v>
       </c>
-      <c r="C15" s="39"/>
+      <c r="C15" s="40"/>
     </row>
     <row r="16" spans="1:3" ht="26.25" thickBot="1">
-      <c r="A16" s="38" t="s">
+      <c r="A16" s="42" t="s">
         <v>26</v>
       </c>
       <c r="B16" s="4" t="s">
@@ -3426,8 +4096,8 @@
         <v>116</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="26.25" thickBot="1">
-      <c r="A17" s="42"/>
+    <row r="17" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A17" s="43"/>
       <c r="B17" s="4" t="s">
         <v>29</v>
       </c>
@@ -3435,8 +4105,8 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="51.75" thickBot="1">
-      <c r="A18" s="42"/>
+    <row r="18" spans="1:3" ht="26.25" thickBot="1">
+      <c r="A18" s="43"/>
       <c r="B18" s="4" t="s">
         <v>31</v>
       </c>
@@ -3445,7 +4115,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" ht="26.25" thickBot="1">
-      <c r="A19" s="42"/>
+      <c r="A19" s="43"/>
       <c r="B19" s="4" t="s">
         <v>33</v>
       </c>
@@ -3454,7 +4124,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" ht="26.25" thickBot="1">
-      <c r="A20" s="42"/>
+      <c r="A20" s="43"/>
       <c r="B20" s="4" t="s">
         <v>34</v>
       </c>
@@ -3463,7 +4133,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" ht="26.25" thickBot="1">
-      <c r="A21" s="42"/>
+      <c r="A21" s="43"/>
       <c r="B21" s="4" t="s">
         <v>35</v>
       </c>
@@ -3472,7 +4142,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" ht="26.25" thickBot="1">
-      <c r="A22" s="40"/>
+      <c r="A22" s="44"/>
       <c r="B22" s="4" t="s">
         <v>36</v>
       </c>
@@ -3480,72 +4150,72 @@
         <v>116</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="230.25" thickBot="1">
-      <c r="A23" s="34" t="s">
+    <row r="23" spans="1:3" ht="39" thickBot="1">
+      <c r="A23" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="39"/>
-      <c r="C23" s="39"/>
-    </row>
-    <row r="24" spans="1:3" ht="77.25" thickBot="1">
-      <c r="A24" s="34" t="s">
+      <c r="B23" s="40"/>
+      <c r="C23" s="40"/>
+    </row>
+    <row r="24" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A24" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="B24" s="39"/>
-      <c r="C24" s="39"/>
-    </row>
-    <row r="25" spans="1:3" ht="64.5" thickBot="1">
-      <c r="A25" s="34" t="s">
+      <c r="B24" s="40"/>
+      <c r="C24" s="40"/>
+    </row>
+    <row r="25" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A25" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="B25" s="39"/>
-      <c r="C25" s="39"/>
-    </row>
-    <row r="26" spans="1:3" ht="141" thickBot="1">
-      <c r="A26" s="34" t="s">
+      <c r="B25" s="40"/>
+      <c r="C25" s="40"/>
+    </row>
+    <row r="26" spans="1:3" ht="26.25" thickBot="1">
+      <c r="A26" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="B26" s="39" t="s">
+      <c r="B26" s="40" t="s">
         <v>100</v>
       </c>
-      <c r="C26" s="39"/>
+      <c r="C26" s="40"/>
     </row>
     <row r="27" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A27" s="41" t="s">
+      <c r="A27" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="B27" s="41"/>
-      <c r="C27" s="41"/>
-    </row>
-    <row r="28" spans="1:3" ht="166.5" thickBot="1">
-      <c r="A28" s="34" t="s">
+      <c r="B27" s="45"/>
+      <c r="C27" s="45"/>
+    </row>
+    <row r="28" spans="1:3" ht="39" thickBot="1">
+      <c r="A28" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="B28" s="39" t="s">
+      <c r="B28" s="40" t="s">
         <v>117</v>
       </c>
-      <c r="C28" s="39"/>
-    </row>
-    <row r="29" spans="1:3" ht="179.25" thickBot="1">
-      <c r="A29" s="34" t="s">
+      <c r="C28" s="40"/>
+    </row>
+    <row r="29" spans="1:3" ht="39" thickBot="1">
+      <c r="A29" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="B29" s="39" t="s">
+      <c r="B29" s="40" t="s">
         <v>99</v>
       </c>
-      <c r="C29" s="39"/>
-    </row>
-    <row r="30" spans="1:3" ht="77.25" thickBot="1">
-      <c r="A30" s="34" t="s">
+      <c r="C29" s="40"/>
+    </row>
+    <row r="30" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A30" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="B30" s="39" t="s">
+      <c r="B30" s="40" t="s">
         <v>118</v>
       </c>
-      <c r="C30" s="39"/>
-    </row>
-    <row r="31" spans="1:3" ht="77.25" thickBot="1">
-      <c r="A31" s="38" t="s">
+      <c r="C30" s="40"/>
+    </row>
+    <row r="31" spans="1:3" ht="26.25" thickBot="1">
+      <c r="A31" s="42" t="s">
         <v>49</v>
       </c>
       <c r="B31" s="4" t="s">
@@ -3555,8 +4225,8 @@
         <v>119</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="77.25" thickBot="1">
-      <c r="A32" s="42"/>
+    <row r="32" spans="1:3" ht="39" thickBot="1">
+      <c r="A32" s="43"/>
       <c r="B32" s="4" t="s">
         <v>51</v>
       </c>
@@ -3564,8 +4234,8 @@
         <v>120</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="39" thickBot="1">
-      <c r="A33" s="42"/>
+    <row r="33" spans="1:3" ht="26.25" thickBot="1">
+      <c r="A33" s="43"/>
       <c r="B33" s="4" t="s">
         <v>52</v>
       </c>
@@ -3574,7 +4244,7 @@
       </c>
     </row>
     <row r="34" spans="1:3" ht="26.25" thickBot="1">
-      <c r="A34" s="42"/>
+      <c r="A34" s="43"/>
       <c r="B34" s="4" t="s">
         <v>53</v>
       </c>
@@ -3582,8 +4252,8 @@
         <v>120</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="39" thickBot="1">
-      <c r="A35" s="42"/>
+    <row r="35" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A35" s="43"/>
       <c r="B35" s="4" t="s">
         <v>54</v>
       </c>
@@ -3591,8 +4261,8 @@
         <v>119</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="39" thickBot="1">
-      <c r="A36" s="42"/>
+    <row r="36" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A36" s="43"/>
       <c r="B36" s="4" t="s">
         <v>55</v>
       </c>
@@ -3600,8 +4270,8 @@
         <v>119</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="26.25" thickBot="1">
-      <c r="A37" s="42"/>
+    <row r="37" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A37" s="43"/>
       <c r="B37" s="4" t="s">
         <v>56</v>
       </c>
@@ -3610,7 +4280,7 @@
       </c>
     </row>
     <row r="38" spans="1:3" ht="26.25" thickBot="1">
-      <c r="A38" s="42"/>
+      <c r="A38" s="43"/>
       <c r="B38" s="4" t="s">
         <v>57</v>
       </c>
@@ -3619,7 +4289,7 @@
       </c>
     </row>
     <row r="39" spans="1:3" ht="26.25" thickBot="1">
-      <c r="A39" s="42"/>
+      <c r="A39" s="43"/>
       <c r="B39" s="4" t="s">
         <v>58</v>
       </c>
@@ -3627,8 +4297,8 @@
         <v>120</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="51.75" thickBot="1">
-      <c r="A40" s="42"/>
+    <row r="40" spans="1:3" ht="26.25" thickBot="1">
+      <c r="A40" s="43"/>
       <c r="B40" s="4" t="s">
         <v>59</v>
       </c>
@@ -3636,8 +4306,8 @@
         <v>120</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="39" thickBot="1">
-      <c r="A41" s="42"/>
+    <row r="41" spans="1:3" ht="26.25" thickBot="1">
+      <c r="A41" s="43"/>
       <c r="B41" s="4" t="s">
         <v>60</v>
       </c>
@@ -3646,7 +4316,7 @@
       </c>
     </row>
     <row r="42" spans="1:3" ht="26.25" thickBot="1">
-      <c r="A42" s="42"/>
+      <c r="A42" s="43"/>
       <c r="B42" s="4" t="s">
         <v>61</v>
       </c>
@@ -3654,8 +4324,8 @@
         <v>120</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="39" thickBot="1">
-      <c r="A43" s="42"/>
+    <row r="43" spans="1:3" ht="26.25" thickBot="1">
+      <c r="A43" s="43"/>
       <c r="B43" s="4" t="s">
         <v>62</v>
       </c>
@@ -3663,8 +4333,8 @@
         <v>120</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="77.25" thickBot="1">
-      <c r="A44" s="42"/>
+    <row r="44" spans="1:3" ht="39" thickBot="1">
+      <c r="A44" s="43"/>
       <c r="B44" s="4" t="s">
         <v>63</v>
       </c>
@@ -3672,8 +4342,8 @@
         <v>119</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="64.5" thickBot="1">
-      <c r="A45" s="42"/>
+    <row r="45" spans="1:3" ht="26.25" thickBot="1">
+      <c r="A45" s="43"/>
       <c r="B45" s="4" t="s">
         <v>64</v>
       </c>
@@ -3682,7 +4352,7 @@
       </c>
     </row>
     <row r="46" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A46" s="42"/>
+      <c r="A46" s="43"/>
       <c r="B46" s="4" t="s">
         <v>65</v>
       </c>
@@ -3691,7 +4361,7 @@
       </c>
     </row>
     <row r="47" spans="1:3" ht="26.25" thickBot="1">
-      <c r="A47" s="42"/>
+      <c r="A47" s="43"/>
       <c r="B47" s="4" t="s">
         <v>66</v>
       </c>
@@ -3700,7 +4370,7 @@
       </c>
     </row>
     <row r="48" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A48" s="42"/>
+      <c r="A48" s="43"/>
       <c r="B48" s="4" t="s">
         <v>67</v>
       </c>
@@ -3708,8 +4378,8 @@
         <v>119</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="39" thickBot="1">
-      <c r="A49" s="42"/>
+    <row r="49" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A49" s="43"/>
       <c r="B49" s="4" t="s">
         <v>68</v>
       </c>
@@ -3718,7 +4388,7 @@
       </c>
     </row>
     <row r="50" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A50" s="42"/>
+      <c r="A50" s="43"/>
       <c r="B50" s="4" t="s">
         <v>69</v>
       </c>
@@ -3727,7 +4397,7 @@
       </c>
     </row>
     <row r="51" spans="1:3" ht="26.25" thickBot="1">
-      <c r="A51" s="42"/>
+      <c r="A51" s="43"/>
       <c r="B51" s="4" t="s">
         <v>70</v>
       </c>
@@ -3735,8 +4405,8 @@
         <v>120</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="115.5" thickBot="1">
-      <c r="A52" s="42"/>
+    <row r="52" spans="1:3" ht="39" thickBot="1">
+      <c r="A52" s="43"/>
       <c r="B52" s="4" t="s">
         <v>71</v>
       </c>
@@ -3745,7 +4415,7 @@
       </c>
     </row>
     <row r="53" spans="1:3" ht="26.25" thickBot="1">
-      <c r="A53" s="42"/>
+      <c r="A53" s="43"/>
       <c r="B53" s="4" t="s">
         <v>72</v>
       </c>
@@ -3753,8 +4423,8 @@
         <v>120</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="77.25" thickBot="1">
-      <c r="A54" s="42"/>
+    <row r="54" spans="1:3" ht="39" thickBot="1">
+      <c r="A54" s="43"/>
       <c r="B54" s="4" t="s">
         <v>73</v>
       </c>
@@ -3763,7 +4433,7 @@
       </c>
     </row>
     <row r="55" spans="1:3" ht="26.25" thickBot="1">
-      <c r="A55" s="42"/>
+      <c r="A55" s="43"/>
       <c r="B55" s="4" t="s">
         <v>74</v>
       </c>
@@ -3771,8 +4441,8 @@
         <v>120</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="51.75" thickBot="1">
-      <c r="A56" s="42"/>
+    <row r="56" spans="1:3" ht="26.25" thickBot="1">
+      <c r="A56" s="43"/>
       <c r="B56" s="4" t="s">
         <v>75</v>
       </c>
@@ -3780,8 +4450,8 @@
         <v>120</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="77.25" thickBot="1">
-      <c r="A57" s="42"/>
+    <row r="57" spans="1:3" ht="39" thickBot="1">
+      <c r="A57" s="43"/>
       <c r="B57" s="4" t="s">
         <v>76</v>
       </c>
@@ -3789,8 +4459,8 @@
         <v>120</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="90" thickBot="1">
-      <c r="A58" s="42"/>
+    <row r="58" spans="1:3" ht="39" thickBot="1">
+      <c r="A58" s="43"/>
       <c r="B58" s="4" t="s">
         <v>77</v>
       </c>
@@ -3798,8 +4468,8 @@
         <v>119</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="77.25" thickBot="1">
-      <c r="A59" s="40"/>
+    <row r="59" spans="1:3" ht="26.25" thickBot="1">
+      <c r="A59" s="44"/>
       <c r="B59" s="4" t="s">
         <v>78</v>
       </c>
@@ -3808,63 +4478,88 @@
       </c>
     </row>
     <row r="60" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A60" s="41" t="s">
+      <c r="A60" s="45" t="s">
         <v>79</v>
       </c>
-      <c r="B60" s="41"/>
-      <c r="C60" s="41"/>
-    </row>
-    <row r="61" spans="1:3" ht="90" thickBot="1">
-      <c r="A61" s="34" t="s">
+      <c r="B60" s="45"/>
+      <c r="C60" s="45"/>
+    </row>
+    <row r="61" spans="1:3" ht="26.25" thickBot="1">
+      <c r="A61" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="B61" s="39"/>
-      <c r="C61" s="39"/>
-    </row>
-    <row r="62" spans="1:3" ht="64.5" thickBot="1">
-      <c r="A62" s="34" t="s">
+      <c r="B61" s="40"/>
+      <c r="C61" s="40"/>
+    </row>
+    <row r="62" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A62" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="B62" s="39"/>
-      <c r="C62" s="39"/>
-    </row>
-    <row r="63" spans="1:3" ht="64.5" thickBot="1">
-      <c r="A63" s="34" t="s">
+      <c r="B62" s="40"/>
+      <c r="C62" s="40"/>
+    </row>
+    <row r="63" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A63" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="B63" s="39"/>
-      <c r="C63" s="39"/>
-    </row>
-    <row r="64" spans="1:3" ht="51.75" thickBot="1">
-      <c r="A64" s="34" t="s">
+      <c r="B63" s="40"/>
+      <c r="C63" s="40"/>
+    </row>
+    <row r="64" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A64" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="B64" s="39"/>
-      <c r="C64" s="39"/>
-    </row>
-    <row r="65" spans="1:3" ht="64.5" thickBot="1">
-      <c r="A65" s="34" t="s">
+      <c r="B64" s="40"/>
+      <c r="C64" s="40"/>
+    </row>
+    <row r="65" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A65" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="B65" s="39"/>
-      <c r="C65" s="39"/>
+      <c r="B65" s="40"/>
+      <c r="C65" s="40"/>
     </row>
     <row r="66" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A66" s="36" t="s">
+      <c r="A66" s="41" t="s">
         <v>85</v>
       </c>
-      <c r="B66" s="36"/>
-      <c r="C66" s="36"/>
-    </row>
-    <row r="67" spans="1:3" ht="102">
-      <c r="A67" s="34" t="s">
+      <c r="B66" s="41"/>
+      <c r="C66" s="41"/>
+    </row>
+    <row r="67" spans="1:3" ht="25.5">
+      <c r="A67" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="B67" s="32"/>
-      <c r="C67" s="32"/>
+      <c r="B67" s="19"/>
+      <c r="C67" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="A16:A22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
     <mergeCell ref="B65:C65"/>
     <mergeCell ref="A66:C66"/>
     <mergeCell ref="A31:A59"/>
@@ -3873,38 +4568,13 @@
     <mergeCell ref="B62:C62"/>
     <mergeCell ref="B63:C63"/>
     <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="A16:A22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD5A0A31-4659-4F09-8CE9-8D259D23E780}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>